<commit_message>
Remove anchor feature prioritization in feature selection
Co-authored-by: sxtdaily <sxtdaily@gmail.com>
</commit_message>
<xml_diff>
--- a/results/results_cox.xlsx
+++ b/results/results_cox.xlsx
@@ -661,17 +661,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0.582 (nan, nan)</t>
+          <t>0.599 (nan, nan)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.667 (nan, nan)</t>
+          <t>0.567 (nan, nan)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.526 (nan, nan)</t>
+          <t>0.593 (nan, nan)</t>
         </is>
       </c>
     </row>
@@ -683,17 +683,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0.505 (nan, nan)</t>
+          <t>0.589 (nan, nan)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
+          <t>0.600 (nan, nan)</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
           <t>0.533 (nan, nan)</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>0.489 (nan, nan)</t>
         </is>
       </c>
     </row>
@@ -705,7 +705,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>0.542 (nan, nan)</t>
+          <t>0.552 (nan, nan)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -715,7 +715,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.541 (nan, nan)</t>
+          <t>0.563 (nan, nan)</t>
         </is>
       </c>
     </row>
@@ -727,7 +727,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>0.595 (nan, nan)</t>
+          <t>0.599 (nan, nan)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -737,7 +737,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.556 (nan, nan)</t>
+          <t>0.607 (nan, nan)</t>
         </is>
       </c>
     </row>
@@ -749,12 +749,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>0.505 (nan, nan)</t>
+          <t>0.532 (nan, nan)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>0.533 (nan, nan)</t>
+          <t>0.667 (nan, nan)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -771,7 +771,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>0.569 (nan, nan)</t>
+          <t>0.612 (nan, nan)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.541 (nan, nan)</t>
+          <t>0.533 (nan, nan)</t>
         </is>
       </c>
     </row>

</xml_diff>